<commit_message>
Changes made ti niva for parallel evaluation.
</commit_message>
<xml_diff>
--- a/Separator Model/Input/niba_V2.xlsx
+++ b/Separator Model/Input/niba_V2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd1a17303fcb2a19/Documentos/RWTH/Semester 4 (SS25)/MA/Modelle/(Model-3)_Separator.py-master/Separator Model/Input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\public\03 Studenten\00 Ausgeschieden\Ivan Guzman\05_Simulations\Abscheidermodell\MA\MA-Model_3\Separator Model\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="101" documentId="8_{3D94B314-A0E8-4B85-9ECF-1D48EFF7D7E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{53E7B3BC-6974-47AC-972D-05F3F5403CD4}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C8FE63A-312D-4863-A1DE-1E9133DEB359}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{E05DA534-964F-48A7-BAA6-64E8E844F20B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E05DA534-964F-48A7-BAA6-64E8E844F20B}"/>
   </bookViews>
   <sheets>
     <sheet name="DataSim" sheetId="1" r:id="rId1"/>
@@ -616,48 +616,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Akzent1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akzent2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akzent3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Akzent4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Akzent5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Akzent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Ausgabe" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Berechnung" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Eingabe" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Ergebnis" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Erklärender Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Gut" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
-    <cellStyle name="Notiz" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Schlecht" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
-    <cellStyle name="Überschrift" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Überschrift 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Überschrift 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Überschrift 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Überschrift 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Warnender Text" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Zelle überprüfen" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -673,9 +673,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 – 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -713,7 +713,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 – 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -819,7 +819,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 – 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -961,7 +961,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -975,7 +975,7 @@
       <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.5703125" customWidth="1"/>
     <col min="2" max="2" width="11.7109375" customWidth="1"/>
@@ -1011,7 +1011,7 @@
       <selection activeCell="D7" sqref="A2:D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1039,10 +1039,10 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="174" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="3" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" customWidth="1"/>
@@ -1108,13 +1108,13 @@
         <v>8.2199999999999999E-3</v>
       </c>
       <c r="G2">
-        <v>0.25</v>
+        <v>0.42857000000000001</v>
       </c>
       <c r="H2">
-        <v>240</v>
+        <v>1500</v>
       </c>
       <c r="I2">
-        <v>1.4189999999999999E-3</v>
+        <v>6.0749999999999997E-4</v>
       </c>
       <c r="J2">
         <v>2.6865E-2</v>

</xml_diff>